<commit_message>
Completed Database and Insert Statements
This is the completion of the creation and insert statements. Also included are the data dictionaries (Xlsx and Html formats) and the latest version of the ERD. Please Read the Readme before marking this assignment
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd2a091fe8f62e20/ARA/2019S1/DBM/Assignment1/DBAssignment2019-S1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="6_{14FCC748-63C1-41F8-A97B-9D7252AB6AD2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{6BCE1C9D-B8DD-4BD5-B689-05989A880D46}"/>
+  <xr:revisionPtr revIDLastSave="170" documentId="6_{14FCC748-63C1-41F8-A97B-9D7252AB6AD2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F7E0B2CE-98D0-4603-8B1B-510DE7C83F18}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{AD730AC6-235C-4820-A77E-31117248BAD0}"/>
+    <workbookView xWindow="727" yWindow="1972" windowWidth="15390" windowHeight="9533" firstSheet="4" activeTab="9" xr2:uid="{AD730AC6-235C-4820-A77E-31117248BAD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Antenna" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="119">
   <si>
     <t>Data Type</t>
   </si>
@@ -237,9 +237,6 @@
     <t>rawArray</t>
   </si>
   <si>
-    <t>VARCHAR(100)</t>
-  </si>
-  <si>
     <t>Raw array of data for the Result</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>signalStrength</t>
   </si>
   <si>
-    <t>DECIMAL(15,12)</t>
-  </si>
-  <si>
     <t>signalLowerThreshold</t>
   </si>
   <si>
@@ -333,9 +327,6 @@
     <t>bluetoothsignal</t>
   </si>
   <si>
-    <t>VARCHAR(15)</t>
-  </si>
-  <si>
     <t>This is the Unique Identifier for the Test. This is a Unique value</t>
   </si>
   <si>
@@ -388,6 +379,24 @@
   </si>
   <si>
     <t>This is used to describe the type of tablet used for the test.</t>
+  </si>
+  <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>This is the generation of test it is.</t>
+  </si>
+  <si>
+    <t>DECIMAL(16,13)</t>
+  </si>
+  <si>
+    <t>VARCHAR(350)</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
   </si>
 </sst>
 </file>
@@ -445,6 +454,30 @@
   </cellStyles>
   <dxfs count="90">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -832,30 +865,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -888,160 +897,160 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E902EB84-473C-47A0-AF45-19A85C4EA433}" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="72" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E902EB84-473C-47A0-AF45-19A85C4EA433}" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="A1:G3" xr:uid="{0CAFE458-CB5E-41A9-876C-EE7333E88566}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{33E259F0-0994-47A7-AF89-8C01E3816066}" name="Name" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{145A5D0D-3965-4E40-871F-BAB7F490D9A2}" name="Data Type" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{3E094563-0105-46A0-B494-97C344BB6007}" name="Not Nullable" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{B39F5866-8901-4A39-9F22-78FDA3E0DBBB}" name="PK" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{41D7BB9A-9F17-4D3C-8351-29A7083D4122}" name="FK" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{D5F82BED-AB68-4531-8DF2-5433F2BACA63}" name="Default" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{98C8D286-D2CF-4FEB-927B-604E91146AF3}" name="Comment" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{33E259F0-0994-47A7-AF89-8C01E3816066}" name="Name" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{145A5D0D-3965-4E40-871F-BAB7F490D9A2}" name="Data Type" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{3E094563-0105-46A0-B494-97C344BB6007}" name="Not Nullable" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{B39F5866-8901-4A39-9F22-78FDA3E0DBBB}" name="PK" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{41D7BB9A-9F17-4D3C-8351-29A7083D4122}" name="FK" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{D5F82BED-AB68-4531-8DF2-5433F2BACA63}" name="Default" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{98C8D286-D2CF-4FEB-927B-604E91146AF3}" name="Comment" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B03B3598-7FAD-4D3B-8EBD-40019A6AA31B}" name="Table10" displayName="Table10" ref="A1:G4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B03B3598-7FAD-4D3B-8EBD-40019A6AA31B}" name="Table10" displayName="Table10" ref="A1:G4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G4" xr:uid="{B4D3B69B-FECF-482E-AC8D-7D02607CC5E2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7606B7C7-7B33-403E-A6E5-DA202FF67E18}" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{390A503D-4CE1-40B9-9D5E-CB59993314FF}" name="Data Type" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{54116E78-E3E8-4D7F-BF3D-957750098139}" name="Not Nullable" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7F21CD68-7EA2-4F11-A271-F1D730540FC9}" name="PK" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{8A49A183-3396-44E3-9D66-EA8BFCFBFB3B}" name="FK" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{0F5EC959-546B-4F05-9BDD-8A74803E95BA}" name="Default" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{71B88348-D2DF-437C-B1F6-6C1FE9087D35}" name="Comment" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7606B7C7-7B33-403E-A6E5-DA202FF67E18}" name="Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{390A503D-4CE1-40B9-9D5E-CB59993314FF}" name="Data Type" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{54116E78-E3E8-4D7F-BF3D-957750098139}" name="Not Nullable" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7F21CD68-7EA2-4F11-A271-F1D730540FC9}" name="PK" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{8A49A183-3396-44E3-9D66-EA8BFCFBFB3B}" name="FK" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{0F5EC959-546B-4F05-9BDD-8A74803E95BA}" name="Default" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{71B88348-D2DF-437C-B1F6-6C1FE9087D35}" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{66C773E6-F5DD-41BD-BFD5-41BC3AE58E0A}" name="Table5" displayName="Table5" ref="A1:G3" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{66C773E6-F5DD-41BD-BFD5-41BC3AE58E0A}" name="Table5" displayName="Table5" ref="A1:G3" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <autoFilter ref="A1:G3" xr:uid="{5722FE1D-6F77-487C-BC90-EE53BB5A78C1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FDFF5878-8B5D-4742-BB70-92A1AF28BA37}" name="Name" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{9AC498B0-5249-458A-879F-57E0C6E0C958}" name="Data Type" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{CCB842FD-B21F-485D-934D-9969C5FBA0DC}" name="Not Nullable" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{8FDA11C0-00C4-49D6-BAE1-4781E48A567C}" name="PK" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{389CFFFA-BFA5-4E4C-AC9B-E1F0235FF675}" name="FK" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{9FDB6397-12F6-45EC-8CBF-EC98F5C6D0FB}" name="Default" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{A9A1145F-53D2-42E1-91AE-41A513D5E16A}" name="Comment" dataDxfId="81"/>
+    <tableColumn id="1" xr3:uid="{FDFF5878-8B5D-4742-BB70-92A1AF28BA37}" name="Name" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{9AC498B0-5249-458A-879F-57E0C6E0C958}" name="Data Type" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{CCB842FD-B21F-485D-934D-9969C5FBA0DC}" name="Not Nullable" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{8FDA11C0-00C4-49D6-BAE1-4781E48A567C}" name="PK" dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{389CFFFA-BFA5-4E4C-AC9B-E1F0235FF675}" name="FK" dataDxfId="74"/>
+    <tableColumn id="6" xr3:uid="{9FDB6397-12F6-45EC-8CBF-EC98F5C6D0FB}" name="Default" dataDxfId="73"/>
+    <tableColumn id="7" xr3:uid="{A9A1145F-53D2-42E1-91AE-41A513D5E16A}" name="Comment" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E4DB7BC-BF16-4E6A-9057-056373B94E30}" name="Table3" displayName="Table3" ref="A1:G2" totalsRowShown="0" headerRowDxfId="54" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9E4DB7BC-BF16-4E6A-9057-056373B94E30}" name="Table3" displayName="Table3" ref="A1:G2" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="A1:G2" xr:uid="{5DE5CD9D-F78B-4BFE-8AFC-7044075EDB2D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0701F233-B2E7-4020-95EE-45D7048DF155}" name="Name" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{2E4A8F89-6EFE-4B21-82F3-FD676F501405}" name="Data Type" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{73B59000-62ED-4A1C-B1F0-8D6E1A2F3607}" name="Not Nullable" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{E31B3F57-478E-453D-ABB1-E13FE2D929EC}" name="PK" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{AE57092F-5A19-449E-B4B7-5BB1A43874F0}" name="FK" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{071D8672-0822-486E-88E4-B5F734741A47}" name="Default" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{FF3528DD-2B1E-4DC2-BADB-C813991A8012}" name="Comment" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{0701F233-B2E7-4020-95EE-45D7048DF155}" name="Name" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{2E4A8F89-6EFE-4B21-82F3-FD676F501405}" name="Data Type" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{73B59000-62ED-4A1C-B1F0-8D6E1A2F3607}" name="Not Nullable" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{E31B3F57-478E-453D-ABB1-E13FE2D929EC}" name="PK" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{AE57092F-5A19-449E-B4B7-5BB1A43874F0}" name="FK" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{071D8672-0822-486E-88E4-B5F734741A47}" name="Default" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{FF3528DD-2B1E-4DC2-BADB-C813991A8012}" name="Comment" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96A8D978-5C00-4E4C-8848-8561076E5BE8}" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0" headerRowDxfId="63" dataDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{96A8D978-5C00-4E4C-8848-8561076E5BE8}" name="Table2" displayName="Table2" ref="A1:G9" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <autoFilter ref="A1:G9" xr:uid="{14E4F528-B018-4EEE-AD25-54677935098D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{332BF98C-5783-4E9D-9879-99CBA9745EAE}" name="Name" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{35D42CE9-F3C2-4A79-84BC-CEC4380B8682}" name="Data Type" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{153203EE-A43D-4757-AC0B-939576A395A4}" name="Not Nullable" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{BFE5A4E8-1D3F-4745-92CC-AC604E96E37F}" name="PK" dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{8DDBF097-692B-45FA-A3B1-C2094CCD2F9A}" name="FK" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{93D7F594-0698-45F5-AB86-CE822BE23DC3}" name="Default" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{E1FC6816-8FEB-45A2-9283-0248D1DA1EDA}" name="Comment" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{332BF98C-5783-4E9D-9879-99CBA9745EAE}" name="Name" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{35D42CE9-F3C2-4A79-84BC-CEC4380B8682}" name="Data Type" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{153203EE-A43D-4757-AC0B-939576A395A4}" name="Not Nullable" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{BFE5A4E8-1D3F-4745-92CC-AC604E96E37F}" name="PK" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{8DDBF097-692B-45FA-A3B1-C2094CCD2F9A}" name="FK" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{93D7F594-0698-45F5-AB86-CE822BE23DC3}" name="Default" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{E1FC6816-8FEB-45A2-9283-0248D1DA1EDA}" name="Comment" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{431F7FC8-AF01-4AE6-85F2-6316D272273E}" name="Table4" displayName="Table4" ref="A1:G3" totalsRowShown="0" headerRowDxfId="45" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{431F7FC8-AF01-4AE6-85F2-6316D272273E}" name="Table4" displayName="Table4" ref="A1:G3" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A1:G3" xr:uid="{333C13C2-0879-439F-B916-0216B0475BF2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4D82FAFF-7431-4134-BD38-B564C8F077E3}" name="Name" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{0CEC33EA-FD84-4BF6-8890-0E7FF041BE2D}" name="Data Type" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{E922DACA-E367-4EFA-9529-E18A235F2400}" name="Not Nullable" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{E574295B-2793-4842-BC7E-4D44623622D1}" name="PK" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{E04C76F3-71E0-40AA-AAC0-9807C1F58819}" name="FK" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{665C83A4-4E39-42B6-AC2B-3F8459F05F04}" name="Default" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{4CC411AA-70B1-43BD-8C2B-D8E7EDA9D0B4}" name="Comment" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{4D82FAFF-7431-4134-BD38-B564C8F077E3}" name="Name" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{0CEC33EA-FD84-4BF6-8890-0E7FF041BE2D}" name="Data Type" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{E922DACA-E367-4EFA-9529-E18A235F2400}" name="Not Nullable" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{E574295B-2793-4842-BC7E-4D44623622D1}" name="PK" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{E04C76F3-71E0-40AA-AAC0-9807C1F58819}" name="FK" dataDxfId="47"/>
+    <tableColumn id="6" xr3:uid="{665C83A4-4E39-42B6-AC2B-3F8459F05F04}" name="Default" dataDxfId="46"/>
+    <tableColumn id="7" xr3:uid="{4CC411AA-70B1-43BD-8C2B-D8E7EDA9D0B4}" name="Comment" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3B0D8CB-A4B7-425E-96A1-49BAC60BDE69}" name="Table6" displayName="Table6" ref="A1:G11" totalsRowShown="0" headerRowDxfId="36" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3B0D8CB-A4B7-425E-96A1-49BAC60BDE69}" name="Table6" displayName="Table6" ref="A1:G11" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:G11" xr:uid="{261D8AA5-A082-492E-831D-EA9150B60DEA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B1539051-5434-4996-9204-79D4F3473517}" name="Name" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{335585DE-0F0A-47AF-8C2D-1D60C7E084B6}" name="Data Type" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{36B0399B-6136-4B4F-884E-7B445E9E1CD6}" name="Not Nullable" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{9BC04FF8-8EE9-42BE-938E-E97A3294A7A1}" name="PK" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{0CDF2621-8AA4-497B-B68D-3B97610758CC}" name="FK" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{2A1FA0C4-1C70-4F6C-9EDE-2EA8C4AD8BA5}" name="Default" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{0E4972C2-0670-4102-83AC-C6AA80E1E17A}" name="Comment" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{B1539051-5434-4996-9204-79D4F3473517}" name="Name" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{335585DE-0F0A-47AF-8C2D-1D60C7E084B6}" name="Data Type" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{36B0399B-6136-4B4F-884E-7B445E9E1CD6}" name="Not Nullable" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{9BC04FF8-8EE9-42BE-938E-E97A3294A7A1}" name="PK" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{0CDF2621-8AA4-497B-B68D-3B97610758CC}" name="FK" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{2A1FA0C4-1C70-4F6C-9EDE-2EA8C4AD8BA5}" name="Default" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{0E4972C2-0670-4102-83AC-C6AA80E1E17A}" name="Comment" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D6E1A107-355D-4447-B450-E22C7A39C656}" name="Table7" displayName="Table7" ref="A1:G7" totalsRowShown="0" headerRowDxfId="27" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D6E1A107-355D-4447-B450-E22C7A39C656}" name="Table7" displayName="Table7" ref="A1:G7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:G7" xr:uid="{A56EB0B2-CC1F-4B87-AF57-AAF51382F91A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{86596568-5F59-48E6-B5A2-FCE7420D5403}" name="Name" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{28A28CEA-F67A-4EE2-82CA-3DE3E06CC012}" name="Data Type" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{5370987C-A823-4F94-B44E-0F309DF961EC}" name="Not Nullable" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{87ADD6D2-2488-4184-88D4-D22E69C3D6D3}" name="PK" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{218B8820-7BF1-46B1-820C-14273152A64C}" name="FK" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{294F63FA-88B3-45C0-ABC1-6CD80426014C}" name="Default" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{5BA01755-ED72-4394-8CBB-08877F1C5020}" name="Comment" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{86596568-5F59-48E6-B5A2-FCE7420D5403}" name="Name" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{28A28CEA-F67A-4EE2-82CA-3DE3E06CC012}" name="Data Type" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{5370987C-A823-4F94-B44E-0F309DF961EC}" name="Not Nullable" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{87ADD6D2-2488-4184-88D4-D22E69C3D6D3}" name="PK" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{218B8820-7BF1-46B1-820C-14273152A64C}" name="FK" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{294F63FA-88B3-45C0-ABC1-6CD80426014C}" name="Default" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{5BA01755-ED72-4394-8CBB-08877F1C5020}" name="Comment" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84B30CC3-2819-48E8-923F-73CFD3E458CE}" name="Table8" displayName="Table8" ref="A1:G3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
-  <autoFilter ref="A1:G3" xr:uid="{983208D5-C2BA-48D2-8124-AA9F23725593}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{84B30CC3-2819-48E8-923F-73CFD3E458CE}" name="Table8" displayName="Table8" ref="A1:G5" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A1:G5" xr:uid="{983208D5-C2BA-48D2-8124-AA9F23725593}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EDDAC676-01E0-440F-93A5-F4EC11501C42}" name="Name" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{4DF22031-F35E-4E06-B44E-CB67FD7DF02C}" name="Data Type" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{DB851A33-8102-4441-92C7-9B869FD52176}" name="Not Nullable" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{AC1A99EE-9484-40D0-AE4C-60B07037D7A7}" name="PK" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{07186570-2394-4A1B-9FAD-FAD127D6D334}" name="FK" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{28346C93-E6F0-401E-9657-E31E5074CC07}" name="Default" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{F3864567-E6D1-40CD-8D39-0A69A23B966C}" name="Comment" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{EDDAC676-01E0-440F-93A5-F4EC11501C42}" name="Name" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{4DF22031-F35E-4E06-B44E-CB67FD7DF02C}" name="Data Type" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{DB851A33-8102-4441-92C7-9B869FD52176}" name="Not Nullable" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{AC1A99EE-9484-40D0-AE4C-60B07037D7A7}" name="PK" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{07186570-2394-4A1B-9FAD-FAD127D6D334}" name="FK" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{28346C93-E6F0-401E-9657-E31E5074CC07}" name="Default" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{F3864567-E6D1-40CD-8D39-0A69A23B966C}" name="Comment" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{32574244-099F-480F-9BF8-60D30960C857}" name="Table9" displayName="Table9" ref="A1:G11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
-  <autoFilter ref="A1:G11" xr:uid="{67DE6B20-F9AE-478E-ACB6-ED6852DD659A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{32574244-099F-480F-9BF8-60D30960C857}" name="Table9" displayName="Table9" ref="A1:G12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:G12" xr:uid="{67DE6B20-F9AE-478E-ACB6-ED6852DD659A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FC842911-6A84-4D8C-B12C-4FEF80CB7EDB}" name="Name" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{6B817C5B-3FA1-400A-9B92-7F3B672CCD4A}" name="Data Type" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{96D5E725-EB1B-4814-90FD-D6579951260C}" name="Not Nullable" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{FA418C70-6B68-42A7-82D2-7966BFA71C27}" name="PK" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{2E5ADF67-722D-4922-B75A-DB46F592674E}" name="FK" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{09E953A6-F599-4556-8483-DB730F206206}" name="Default" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{AB636EC5-DD1F-4C94-B1FD-967EF3423F06}" name="Comment" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{FC842911-6A84-4D8C-B12C-4FEF80CB7EDB}" name="Name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{6B817C5B-3FA1-400A-9B92-7F3B672CCD4A}" name="Data Type" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{96D5E725-EB1B-4814-90FD-D6579951260C}" name="Not Nullable" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{FA418C70-6B68-42A7-82D2-7966BFA71C27}" name="PK" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{2E5ADF67-722D-4922-B75A-DB46F592674E}" name="FK" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{09E953A6-F599-4556-8483-DB730F206206}" name="Default" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{AB636EC5-DD1F-4C94-B1FD-967EF3423F06}" name="Comment" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1350,18 +1359,18 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1384,7 +1393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1405,7 +1414,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -1438,22 +1447,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3DBE75-7CF9-447C-B386-224D9754064E}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="78.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" customWidth="1"/>
+    <col min="4" max="4" width="5.3984375" customWidth="1"/>
+    <col min="5" max="5" width="5.265625" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="78.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1476,9 +1485,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -1494,15 +1503,15 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -1515,15 +1524,15 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
@@ -1536,7 +1545,7 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1552,21 +1561,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="A1:XFD1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="88.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1610,7 +1619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1647,16 +1656,16 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="118.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="13.73046875" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="118.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1712,22 +1721,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE60C6D-FFE8-4914-AAFD-448BEA67D962}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" customWidth="1"/>
-    <col min="7" max="7" width="92.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.3984375" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1328125" customWidth="1"/>
+    <col min="7" max="7" width="92.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1750,7 +1759,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1771,7 +1780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1792,7 +1801,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1813,7 +1822,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1834,7 +1843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1857,7 +1866,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1878,7 +1887,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1899,7 +1908,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
@@ -1934,21 +1943,21 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="A1:XFD1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="91.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="91.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1971,7 +1980,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1992,7 +2001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2025,22 +2034,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FBEEFD-277F-4E42-A7AF-B79D2C344082}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.86328125" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="73.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2063,7 +2072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>49</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2105,7 +2114,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -2189,7 +2198,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
@@ -2210,12 +2219,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>19</v>
@@ -2228,15 +2237,15 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -2249,15 +2258,15 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
@@ -2270,7 +2279,7 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2283,24 +2292,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146B3D67-E5C4-4A2C-80CC-6E1769E9CD51}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.265625" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="76.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="76.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2323,9 +2332,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -2341,12 +2350,12 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
@@ -2362,10 +2371,10 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -2383,15 +2392,15 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>19</v>
@@ -2404,49 +2413,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2459,22 +2426,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69BC563-9A61-4385-BFF8-659317B8498C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.86328125" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="78.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2497,9 +2464,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -2515,12 +2482,12 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>56</v>
@@ -2536,7 +2503,49 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2549,22 +2558,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7BB214-6C67-443D-83B3-9886E517140C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
-    <col min="7" max="7" width="63.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.265625" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
+    <col min="3" max="3" width="18.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" customWidth="1"/>
+    <col min="7" max="7" width="63.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2587,7 +2596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -2605,10 +2614,10 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2626,10 +2635,10 @@
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2647,10 +2656,10 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2668,12 +2677,12 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>22</v>
@@ -2689,15 +2698,15 @@
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -2710,12 +2719,12 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>47</v>
@@ -2724,22 +2733,22 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -2752,15 +2761,15 @@
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>
@@ -2773,15 +2782,15 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
@@ -2794,7 +2803,28 @@
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>